<commit_message>
Test cases and daily reports
</commit_message>
<xml_diff>
--- a/Tests/Product page unit test.xlsx
+++ b/Tests/Product page unit test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Atech Computers Website Test Cases</t>
   </si>
@@ -97,6 +97,15 @@
 2) It will show a list of all products from selected "Category" located below search button from search products page.
 3) It will show a list of all products from selected "Provider" located below search button from search products page.
 4) Change to "a list of products which meet all the keywords is shown.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Add to Cart option is not implemented in this version.</t>
   </si>
 </sst>
 </file>
@@ -483,6 +492,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -527,15 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,7 +863,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,36 +877,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -926,96 +935,108 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="6">
         <v>2</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="6">
         <v>3</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="6">
         <v>4</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="6">
         <v>5</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="10">
         <v>6</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="12"/>
       <c r="H10" s="13"/>
     </row>

</xml_diff>